<commit_message>
commit with VIM yellow test message with red test1 message
</commit_message>
<xml_diff>
--- a/Hearthstone_stats.xlsx
+++ b/Hearthstone_stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
   <si>
     <t>Odd Paladin</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Some changes 1</t>
+  </si>
+  <si>
+    <t>Some changes 3</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,6 +639,11 @@
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>